<commit_message>
Merged Genetic with Fussy algorithms
</commit_message>
<xml_diff>
--- a/Lemonade/Validator.xlsx
+++ b/Lemonade/Validator.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luishernandezayala/Google Drive/Escuela/13 cuatri/AI/LogicaDifusa/Gaussy3DModel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luishernandezayala/Google Drive/Escuela/13 cuatri/AI/LogicaDifusa/Lemonade/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBB30B9-D996-DD44-856F-735896EDC487}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45209DB-1977-1447-AB99-7255A206A1E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{2D690949-DFAD-4B4A-A61E-700375795F76}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19680" xr2:uid="{2D690949-DFAD-4B4A-A61E-700375795F76}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -119,7 +119,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0000000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -212,7 +212,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -532,7 +532,7 @@
   <dimension ref="B1:X58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -671,7 +671,7 @@
         <v>2.9</v>
       </c>
       <c r="N3" s="3">
-        <f t="shared" ref="M2:N4" si="2">$C$11*N$1+$D$11*$K3+$E$11</f>
+        <f t="shared" ref="M3:N4" si="2">$C$11*N$1+$D$11*$K3+$E$11</f>
         <v>2.8</v>
       </c>
       <c r="P3" s="2">
@@ -724,7 +724,7 @@
         <v>2</v>
       </c>
       <c r="L4" s="3">
-        <f t="shared" ref="L3:L4" si="5">$C$11*L$1+$D$11*$K4+$E$11</f>
+        <f t="shared" ref="L4" si="5">$C$11*L$1+$D$11*$K4+$E$11</f>
         <v>6</v>
       </c>
       <c r="M4" s="3">
@@ -1506,7 +1506,7 @@
         <v>9.9280385390811021E-2</v>
       </c>
       <c r="N23" s="3">
-        <f t="shared" ref="M23:N23" si="18">E$2*$C$7</f>
+        <f t="shared" ref="N23" si="18">E$2*$C$7</f>
         <v>9.5228698964597999E-2</v>
       </c>
       <c r="P23" s="2">

</xml_diff>